<commit_message>
Definicion de atributos class reserva
</commit_message>
<xml_diff>
--- a/Diagrama Proyecto Lab 2.xlsx
+++ b/Diagrama Proyecto Lab 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://frgputneduar-my.sharepoint.com/personal/agustin_bernal_alumnos_frgp_utn_edu_ar/Documents/Escritorio/Proyecto LAB II/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aby\Desktop\Repositorio Labo2\Proyecto-Final-LAB-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46199353-4B94-44F2-8B53-9062AFBD8037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0405A8C-DB63-4681-9033-CCBB15B4D2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{114F25F1-BAA8-49DE-8C7A-F4FC53EA1D42}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Menu Principal</t>
   </si>
@@ -177,6 +177,30 @@
   </si>
   <si>
     <t>Menu</t>
+  </si>
+  <si>
+    <t>char _Nombre</t>
+  </si>
+  <si>
+    <t>Fecha _Fecha</t>
+  </si>
+  <si>
+    <t>int  _Numero</t>
+  </si>
+  <si>
+    <t>int  _NumeroMesa</t>
+  </si>
+  <si>
+    <t>Bool _Estado</t>
+  </si>
+  <si>
+    <t>bool _Estado</t>
+  </si>
+  <si>
+    <t>char _NombreCliente</t>
+  </si>
+  <si>
+    <t>int _NumeroPersonas</t>
   </si>
 </sst>
 </file>
@@ -460,12 +484,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -494,55 +516,55 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,7 +907,7 @@
   <dimension ref="A2:Z44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,481 +916,494 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="K2" s="53" t="s">
+      <c r="B2" s="45"/>
+      <c r="K2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
+      <c r="H3" s="25"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="27" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="27" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="K5" s="54" t="s">
+      <c r="H5" s="17"/>
+      <c r="K5" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="N5" s="54" t="s">
+      <c r="L5" s="53"/>
+      <c r="N5" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="54"/>
-      <c r="Q5" s="54" t="s">
+      <c r="O5" s="53"/>
+      <c r="Q5" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="T5" s="54" t="s">
+      <c r="R5" s="53"/>
+      <c r="T5" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="U5" s="54"/>
+      <c r="U5" s="53"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="27" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="6"/>
-      <c r="K6" s="55" t="s">
+      <c r="H6" s="17"/>
+      <c r="I6" s="4"/>
+      <c r="K6" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="56"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="56"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="56"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="56"/>
+      <c r="L6" s="42"/>
+      <c r="N6" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="42"/>
+      <c r="Q6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="42"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="42"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="28" t="s">
+      <c r="B7" s="49"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="K7" s="57" t="s">
+      <c r="H7" s="25"/>
+      <c r="K7" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="57"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="56"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="56"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="56"/>
+      <c r="L7" s="43"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="42"/>
+      <c r="Q7" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="42"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="42"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="28" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="K8" s="57" t="s">
+      <c r="H8" s="25"/>
+      <c r="K8" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="57"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="56"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="56"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="56"/>
+      <c r="L8" s="43"/>
+      <c r="N8" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="42"/>
+      <c r="Q8" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="R8" s="42"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="42"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C9" s="45"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="27" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="K9" s="57" t="s">
+      <c r="H9" s="17"/>
+      <c r="K9" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="57"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="56"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="56"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="56"/>
+      <c r="L9" s="43"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="42"/>
+      <c r="Q9" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" s="42"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="42"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C10" s="45"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="K10" s="57" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="K10" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="57"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="56"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="56"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="56"/>
+      <c r="L10" s="43"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
+      <c r="Q10" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="R10" s="42"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="42"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C11" s="45"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="30" t="s">
+      <c r="C11" s="35"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="K11" s="57" t="s">
+      <c r="H11" s="19"/>
+      <c r="K11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="57"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="56"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="56"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="56"/>
+      <c r="L11" s="43"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="42"/>
+      <c r="Q11" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="R11" s="42"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="42"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C12" s="45"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="9"/>
-      <c r="G12" s="21" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+      <c r="G12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="K12" s="57" t="s">
+      <c r="H12" s="19"/>
+      <c r="K12" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="57"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="56"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="56"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="56"/>
+      <c r="L12" s="43"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="42"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="42"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="42"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C13" s="45"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="9"/>
-      <c r="G13" s="21" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
+      <c r="G13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C14" s="45"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="9"/>
-      <c r="G14" s="22" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+      <c r="G14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C15" s="45"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="9"/>
-      <c r="G15" s="21" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
+      <c r="G15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C16" s="45"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="9"/>
-      <c r="G16" s="21" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7"/>
+      <c r="G16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="45"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="9"/>
-      <c r="G17" s="21" t="s">
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="35"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="G17" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="45"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="9"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="45"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="23" t="s">
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="35"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="35"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="45"/>
-      <c r="D20" s="14"/>
-      <c r="G20" s="23" t="s">
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="35"/>
+      <c r="D20" s="12"/>
+      <c r="G20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="23"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="45"/>
-      <c r="D21" s="14"/>
-      <c r="G21" s="23" t="s">
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="35"/>
+      <c r="D21" s="12"/>
+      <c r="G21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="23"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="45"/>
-      <c r="D22" s="14"/>
-      <c r="G22" s="24" t="s">
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="35"/>
+      <c r="D22" s="12"/>
+      <c r="G22" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="45"/>
-      <c r="D23" s="14"/>
-      <c r="G23" s="23" t="s">
+      <c r="H22" s="29"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="35"/>
+      <c r="D23" s="12"/>
+      <c r="G23" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="45"/>
-      <c r="D24" s="14"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="45"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="33" t="s">
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="35"/>
+      <c r="D24" s="12"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="35"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="34"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="45"/>
-      <c r="G26" s="33" t="s">
+      <c r="H25" s="51"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="35"/>
+      <c r="G26" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="34"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="45"/>
-      <c r="G27" s="33" t="s">
+      <c r="H26" s="51"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="35"/>
+      <c r="G27" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="34"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="45"/>
-      <c r="G28" s="33" t="s">
+      <c r="H27" s="51"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="35"/>
+      <c r="G28" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="34"/>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="45"/>
-      <c r="G29" s="25" t="s">
+      <c r="H28" s="51"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="35"/>
+      <c r="G29" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="45"/>
-      <c r="G30" s="25" t="s">
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="35"/>
+      <c r="G30" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="45"/>
-      <c r="G31" s="25" t="s">
+      <c r="H30" s="23"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="35"/>
+      <c r="G31" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="45"/>
-      <c r="G32" s="25" t="s">
+      <c r="H31" s="23"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="35"/>
+      <c r="G32" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="45"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="32"/>
+      <c r="C33" s="35"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="30"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="45"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="32"/>
+      <c r="C34" s="35"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="30"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="45"/>
-      <c r="G35" s="25" t="s">
+      <c r="C35" s="35"/>
+      <c r="G35" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="25"/>
+      <c r="H35" s="23"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="45"/>
+      <c r="C36" s="35"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="47"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="48" t="s">
+      <c r="C37" s="37"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="H37" s="49"/>
+      <c r="H37" s="55"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G38" s="49" t="s">
+      <c r="G38" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="49"/>
+      <c r="H38" s="55"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G39" s="49" t="s">
+      <c r="G39" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="H39" s="49"/>
+      <c r="H39" s="55"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="49" t="s">
+      <c r="G40" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H40" s="49"/>
+      <c r="H40" s="55"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G41" s="50"/>
-      <c r="H41" s="51"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="39"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G42" s="50"/>
-      <c r="H42" s="51"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G43" s="50"/>
-      <c r="H43" s="51"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="39"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G44" s="50"/>
-      <c r="H44" s="52"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="T5:U5"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G39:H39"/>
@@ -1379,6 +1414,7 @@
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G25:H25"/>
+    <mergeCell ref="T5:U5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A7:B7"/>

</xml_diff>

<commit_message>
creacion del proyecto en codeblock
</commit_message>
<xml_diff>
--- a/Diagrama Proyecto Lab 2.xlsx
+++ b/Diagrama Proyecto Lab 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://frgputneduar-my.sharepoint.com/personal/agustin_bernal_alumnos_frgp_utn_edu_ar/Documents/Escritorio/Proyecto LAB II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{D72C21AE-0112-4E12-ABC5-1399829BE6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CCD8B6-06C5-4C31-8EC1-4331D549F53E}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:1_{D72C21AE-0112-4E12-ABC5-1399829BE6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{372A2EA0-EA6B-441F-B820-E0AB1493EE44}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{114F25F1-BAA8-49DE-8C7A-F4FC53EA1D42}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>Menu Principal</t>
   </si>
@@ -237,6 +237,33 @@
   </si>
   <si>
     <t>MENUS</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>int ID;</t>
+  </si>
+  <si>
+    <t>    bool estado;</t>
+  </si>
+  <si>
+    <t>    int tipo;</t>
+  </si>
+  <si>
+    <t>    char nombre</t>
+  </si>
+  <si>
+    <t>    char apellido</t>
+  </si>
+  <si>
+    <t>    char cuil</t>
+  </si>
+  <si>
+    <t>    char contrasenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Fecha </t>
   </si>
 </sst>
 </file>
@@ -650,39 +677,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -696,23 +690,37 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,11 +737,71 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,6 +811,24 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -761,65 +847,8 @@
     <xf numFmtId="0" fontId="8" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,6 +1051,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1344,7 +1377,7 @@
   <dimension ref="A2:AH62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y63" sqref="Y63"/>
+      <selection activeCell="AE19" sqref="AE19:AH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,28 +1388,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="S2" s="77" t="s">
+      <c r="B2" s="92"/>
+      <c r="S2" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="79"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="74"/>
     </row>
     <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1391,22 +1424,22 @@
         <v>5</v>
       </c>
       <c r="H3" s="25"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="81"/>
-      <c r="U3" s="81"/>
-      <c r="V3" s="81"/>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="81"/>
-      <c r="Z3" s="81"/>
-      <c r="AA3" s="81"/>
-      <c r="AB3" s="81"/>
-      <c r="AC3" s="81"/>
-      <c r="AD3" s="81"/>
-      <c r="AE3" s="81"/>
-      <c r="AF3" s="81"/>
-      <c r="AG3" s="81"/>
-      <c r="AH3" s="82"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
+      <c r="AB3" s="76"/>
+      <c r="AC3" s="76"/>
+      <c r="AD3" s="76"/>
+      <c r="AE3" s="76"/>
+      <c r="AF3" s="76"/>
+      <c r="AG3" s="76"/>
+      <c r="AH3" s="77"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -1435,28 +1468,30 @@
         <v>15</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="S5" s="54" t="s">
+      <c r="S5" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="54"/>
+      <c r="T5" s="78"/>
       <c r="U5" s="27"/>
-      <c r="V5" s="54" t="s">
+      <c r="V5" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="W5" s="54"/>
+      <c r="W5" s="78"/>
       <c r="X5" s="27"/>
-      <c r="Y5" s="54" t="s">
+      <c r="Y5" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="Z5" s="54"/>
+      <c r="Z5" s="78"/>
       <c r="AA5" s="27"/>
-      <c r="AB5" s="54" t="s">
+      <c r="AB5" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="AC5" s="54"/>
+      <c r="AC5" s="78"/>
       <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="27"/>
+      <c r="AE5" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF5" s="78"/>
       <c r="AG5" s="27"/>
       <c r="AH5" s="27"/>
     </row>
@@ -1474,42 +1509,36 @@
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="S6" s="57" t="s">
+      <c r="S6" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="T6" s="58"/>
+      <c r="T6" s="47"/>
       <c r="U6" s="27"/>
-      <c r="V6" s="57" t="s">
+      <c r="V6" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="W6" s="58"/>
+      <c r="W6" s="47"/>
       <c r="X6" s="27"/>
-      <c r="Y6" s="59" t="s">
+      <c r="Y6" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="Z6" s="60"/>
+      <c r="Z6" s="49"/>
       <c r="AA6" s="27"/>
-      <c r="AB6" s="57"/>
-      <c r="AC6" s="58"/>
+      <c r="AB6" s="46"/>
+      <c r="AC6" s="47"/>
       <c r="AD6" s="27"/>
-      <c r="AE6" s="27"/>
-      <c r="AF6" s="27"/>
+      <c r="AE6" s="114" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF6" s="47"/>
       <c r="AG6" s="27"/>
       <c r="AH6" s="27"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="49"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="36"/>
       <c r="D7" s="2"/>
       <c r="E7" s="8"/>
@@ -1518,34 +1547,36 @@
         <v>16</v>
       </c>
       <c r="H7" s="25"/>
-      <c r="S7" s="61" t="s">
+      <c r="S7" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="61"/>
+      <c r="T7" s="50"/>
       <c r="U7" s="27"/>
-      <c r="V7" s="57" t="s">
+      <c r="V7" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="W7" s="58"/>
+      <c r="W7" s="47"/>
       <c r="X7" s="27"/>
-      <c r="Y7" s="102" t="s">
+      <c r="Y7" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="Z7" s="103"/>
+      <c r="Z7" s="62"/>
       <c r="AA7" s="27"/>
-      <c r="AB7" s="57"/>
-      <c r="AC7" s="58"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="47"/>
       <c r="AD7" s="27"/>
-      <c r="AE7" s="27"/>
-      <c r="AF7" s="27"/>
+      <c r="AE7" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF7" s="47"/>
       <c r="AG7" s="27"/>
       <c r="AH7" s="27"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="47"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="35"/>
       <c r="D8" s="2"/>
       <c r="E8" s="8"/>
@@ -1554,26 +1585,28 @@
         <v>9</v>
       </c>
       <c r="H8" s="25"/>
-      <c r="S8" s="61" t="s">
+      <c r="S8" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="T8" s="61"/>
+      <c r="T8" s="50"/>
       <c r="U8" s="27"/>
-      <c r="V8" s="57" t="s">
+      <c r="V8" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="W8" s="58"/>
+      <c r="W8" s="47"/>
       <c r="X8" s="27"/>
-      <c r="Y8" s="62" t="s">
+      <c r="Y8" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="Z8" s="63"/>
+      <c r="Z8" s="52"/>
       <c r="AA8" s="27"/>
-      <c r="AB8" s="57"/>
-      <c r="AC8" s="58"/>
+      <c r="AB8" s="46"/>
+      <c r="AC8" s="47"/>
       <c r="AD8" s="27"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="27"/>
+      <c r="AE8" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF8" s="47"/>
       <c r="AG8" s="27"/>
       <c r="AH8" s="27"/>
     </row>
@@ -1586,26 +1619,28 @@
         <v>17</v>
       </c>
       <c r="H9" s="17"/>
-      <c r="S9" s="61" t="s">
+      <c r="S9" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="T9" s="61"/>
+      <c r="T9" s="50"/>
       <c r="U9" s="27"/>
-      <c r="V9" s="57" t="s">
+      <c r="V9" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="W9" s="58"/>
+      <c r="W9" s="47"/>
       <c r="X9" s="27"/>
-      <c r="Y9" s="57" t="s">
+      <c r="Y9" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="Z9" s="58"/>
+      <c r="Z9" s="47"/>
       <c r="AA9" s="27"/>
-      <c r="AB9" s="57"/>
-      <c r="AC9" s="58"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="47"/>
       <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27"/>
+      <c r="AE9" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF9" s="47"/>
       <c r="AG9" s="27"/>
       <c r="AH9" s="27"/>
     </row>
@@ -1616,26 +1651,28 @@
       <c r="F10" s="9"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
-      <c r="S10" s="61" t="s">
+      <c r="S10" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="61"/>
+      <c r="T10" s="50"/>
       <c r="U10" s="27"/>
-      <c r="V10" s="64" t="s">
+      <c r="V10" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="W10" s="65"/>
+      <c r="W10" s="54"/>
       <c r="X10" s="27"/>
-      <c r="Y10" s="57" t="s">
+      <c r="Y10" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="Z10" s="58"/>
+      <c r="Z10" s="47"/>
       <c r="AA10" s="27"/>
-      <c r="AB10" s="57"/>
-      <c r="AC10" s="58"/>
+      <c r="AB10" s="46"/>
+      <c r="AC10" s="47"/>
       <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
+      <c r="AE10" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF10" s="47"/>
       <c r="AG10" s="27"/>
       <c r="AH10" s="27"/>
     </row>
@@ -1648,24 +1685,26 @@
         <v>10</v>
       </c>
       <c r="H11" s="19"/>
-      <c r="S11" s="55" t="s">
+      <c r="S11" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="55"/>
+      <c r="T11" s="44"/>
       <c r="U11" s="27"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="58"/>
+      <c r="V11" s="46"/>
+      <c r="W11" s="47"/>
       <c r="X11" s="27"/>
-      <c r="Y11" s="66" t="s">
+      <c r="Y11" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="Z11" s="67"/>
+      <c r="Z11" s="56"/>
       <c r="AA11" s="27"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="58"/>
+      <c r="AB11" s="46"/>
+      <c r="AC11" s="47"/>
       <c r="AD11" s="27"/>
-      <c r="AE11" s="27"/>
-      <c r="AF11" s="27"/>
+      <c r="AE11" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF11" s="47"/>
       <c r="AG11" s="27"/>
       <c r="AH11" s="27"/>
     </row>
@@ -1677,22 +1716,24 @@
         <v>11</v>
       </c>
       <c r="H12" s="19"/>
-      <c r="S12" s="56" t="s">
+      <c r="S12" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="T12" s="56"/>
+      <c r="T12" s="45"/>
       <c r="U12" s="27"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="58"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="47"/>
       <c r="X12" s="27"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="58"/>
+      <c r="Y12" s="46"/>
+      <c r="Z12" s="47"/>
       <c r="AA12" s="27"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="58"/>
+      <c r="AB12" s="46"/>
+      <c r="AC12" s="47"/>
       <c r="AD12" s="27"/>
-      <c r="AE12" s="27"/>
-      <c r="AF12" s="27"/>
+      <c r="AE12" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF12" s="47"/>
       <c r="AG12" s="27"/>
       <c r="AH12" s="27"/>
     </row>
@@ -1716,9 +1757,10 @@
       <c r="AB13" s="27"/>
       <c r="AC13" s="27"/>
       <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
+      <c r="AE13" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF13" s="47"/>
       <c r="AH13" s="27"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -1754,24 +1796,24 @@
         <v>12</v>
       </c>
       <c r="H15" s="19"/>
-      <c r="S15" s="77" t="s">
+      <c r="S15" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="T15" s="78"/>
-      <c r="U15" s="78"/>
-      <c r="V15" s="78"/>
-      <c r="W15" s="78"/>
-      <c r="X15" s="78"/>
-      <c r="Y15" s="78"/>
-      <c r="Z15" s="78"/>
-      <c r="AA15" s="78"/>
-      <c r="AB15" s="78"/>
-      <c r="AC15" s="78"/>
-      <c r="AD15" s="78"/>
-      <c r="AE15" s="78"/>
-      <c r="AF15" s="78"/>
-      <c r="AG15" s="78"/>
-      <c r="AH15" s="79"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="73"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="73"/>
+      <c r="X15" s="73"/>
+      <c r="Y15" s="73"/>
+      <c r="Z15" s="73"/>
+      <c r="AA15" s="73"/>
+      <c r="AB15" s="73"/>
+      <c r="AC15" s="73"/>
+      <c r="AD15" s="73"/>
+      <c r="AE15" s="73"/>
+      <c r="AF15" s="73"/>
+      <c r="AG15" s="73"/>
+      <c r="AH15" s="74"/>
     </row>
     <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="35"/>
@@ -1781,22 +1823,22 @@
         <v>13</v>
       </c>
       <c r="H16" s="19"/>
-      <c r="S16" s="80"/>
-      <c r="T16" s="81"/>
-      <c r="U16" s="81"/>
-      <c r="V16" s="81"/>
-      <c r="W16" s="81"/>
-      <c r="X16" s="81"/>
-      <c r="Y16" s="81"/>
-      <c r="Z16" s="81"/>
-      <c r="AA16" s="81"/>
-      <c r="AB16" s="81"/>
-      <c r="AC16" s="81"/>
-      <c r="AD16" s="81"/>
-      <c r="AE16" s="81"/>
-      <c r="AF16" s="81"/>
-      <c r="AG16" s="81"/>
-      <c r="AH16" s="82"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="76"/>
+      <c r="U16" s="76"/>
+      <c r="V16" s="76"/>
+      <c r="W16" s="76"/>
+      <c r="X16" s="76"/>
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="76"/>
+      <c r="AA16" s="76"/>
+      <c r="AB16" s="76"/>
+      <c r="AC16" s="76"/>
+      <c r="AD16" s="76"/>
+      <c r="AE16" s="76"/>
+      <c r="AF16" s="76"/>
+      <c r="AG16" s="76"/>
+      <c r="AH16" s="77"/>
     </row>
     <row r="17" spans="3:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="35"/>
@@ -1806,30 +1848,30 @@
         <v>17</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="S17" s="83" t="s">
+      <c r="S17" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="T17" s="83"/>
-      <c r="U17" s="83"/>
-      <c r="V17" s="83"/>
-      <c r="W17" s="83" t="s">
+      <c r="T17" s="97"/>
+      <c r="U17" s="97"/>
+      <c r="V17" s="97"/>
+      <c r="W17" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="X17" s="83"/>
-      <c r="Y17" s="83"/>
-      <c r="Z17" s="83"/>
-      <c r="AA17" s="83" t="s">
+      <c r="X17" s="97"/>
+      <c r="Y17" s="97"/>
+      <c r="Z17" s="97"/>
+      <c r="AA17" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="AB17" s="83"/>
-      <c r="AC17" s="83"/>
-      <c r="AD17" s="83"/>
-      <c r="AE17" s="83" t="s">
+      <c r="AB17" s="97"/>
+      <c r="AC17" s="97"/>
+      <c r="AD17" s="97"/>
+      <c r="AE17" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="AF17" s="83"/>
-      <c r="AG17" s="83"/>
-      <c r="AH17" s="83"/>
+      <c r="AF17" s="97"/>
+      <c r="AG17" s="97"/>
+      <c r="AH17" s="97"/>
     </row>
     <row r="18" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C18" s="35"/>
@@ -1837,18 +1879,18 @@
       <c r="E18" s="7"/>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
-      <c r="S18" s="73"/>
+      <c r="S18" s="57"/>
       <c r="W18" s="41"/>
-      <c r="AA18" s="84" t="s">
+      <c r="AA18" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="AB18" s="85"/>
-      <c r="AC18" s="85"/>
-      <c r="AD18" s="86"/>
-      <c r="AE18" s="68"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="70"/>
+      <c r="AB18" s="100"/>
+      <c r="AC18" s="100"/>
+      <c r="AD18" s="101"/>
+      <c r="AE18" s="85"/>
+      <c r="AF18" s="86"/>
+      <c r="AG18" s="86"/>
+      <c r="AH18" s="87"/>
     </row>
     <row r="19" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C19" s="35"/>
@@ -1860,23 +1902,23 @@
       </c>
       <c r="H19" s="21"/>
       <c r="S19" s="41"/>
-      <c r="T19" s="76"/>
-      <c r="U19" s="76"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="60"/>
       <c r="V19" s="42"/>
-      <c r="W19" s="68"/>
-      <c r="X19" s="69"/>
-      <c r="Y19" s="69"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="106" t="s">
+      <c r="W19" s="85"/>
+      <c r="X19" s="86"/>
+      <c r="Y19" s="86"/>
+      <c r="Z19" s="87"/>
+      <c r="AA19" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="AB19" s="104"/>
-      <c r="AC19" s="104"/>
-      <c r="AD19" s="105"/>
-      <c r="AE19" s="68"/>
-      <c r="AF19" s="69"/>
-      <c r="AG19" s="69"/>
-      <c r="AH19" s="70"/>
+      <c r="AB19" s="82"/>
+      <c r="AC19" s="82"/>
+      <c r="AD19" s="83"/>
+      <c r="AE19" s="85"/>
+      <c r="AF19" s="86"/>
+      <c r="AG19" s="86"/>
+      <c r="AH19" s="87"/>
     </row>
     <row r="20" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C20" s="35"/>
@@ -1885,24 +1927,24 @@
         <v>19</v>
       </c>
       <c r="H20" s="21"/>
-      <c r="S20" s="68"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="70"/>
-      <c r="W20" s="68"/>
-      <c r="X20" s="69"/>
-      <c r="Y20" s="69"/>
-      <c r="Z20" s="70"/>
-      <c r="AA20" s="87" t="s">
+      <c r="S20" s="85"/>
+      <c r="T20" s="86"/>
+      <c r="U20" s="86"/>
+      <c r="V20" s="87"/>
+      <c r="W20" s="85"/>
+      <c r="X20" s="86"/>
+      <c r="Y20" s="86"/>
+      <c r="Z20" s="87"/>
+      <c r="AA20" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="AB20" s="88"/>
-      <c r="AC20" s="88"/>
-      <c r="AD20" s="89"/>
-      <c r="AE20" s="68"/>
-      <c r="AF20" s="69"/>
-      <c r="AG20" s="69"/>
-      <c r="AH20" s="70"/>
+      <c r="AB20" s="109"/>
+      <c r="AC20" s="109"/>
+      <c r="AD20" s="110"/>
+      <c r="AE20" s="85"/>
+      <c r="AF20" s="86"/>
+      <c r="AG20" s="86"/>
+      <c r="AH20" s="87"/>
     </row>
     <row r="21" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C21" s="35"/>
@@ -1911,22 +1953,22 @@
         <v>20</v>
       </c>
       <c r="H21" s="21"/>
-      <c r="S21" s="71"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="68"/>
-      <c r="X21" s="69"/>
-      <c r="Y21" s="69"/>
-      <c r="Z21" s="70"/>
-      <c r="AA21" s="68"/>
-      <c r="AB21" s="69"/>
-      <c r="AC21" s="69"/>
-      <c r="AD21" s="70"/>
-      <c r="AE21" s="68"/>
-      <c r="AF21" s="69"/>
-      <c r="AG21" s="69"/>
-      <c r="AH21" s="70"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="85"/>
+      <c r="X21" s="86"/>
+      <c r="Y21" s="86"/>
+      <c r="Z21" s="87"/>
+      <c r="AA21" s="85"/>
+      <c r="AB21" s="86"/>
+      <c r="AC21" s="86"/>
+      <c r="AD21" s="87"/>
+      <c r="AE21" s="85"/>
+      <c r="AF21" s="86"/>
+      <c r="AG21" s="86"/>
+      <c r="AH21" s="87"/>
     </row>
     <row r="22" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C22" s="35"/>
@@ -1936,20 +1978,20 @@
       </c>
       <c r="H22" s="29"/>
       <c r="S22" s="41"/>
-      <c r="W22" s="93" t="s">
+      <c r="W22" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="X22" s="94"/>
-      <c r="Y22" s="94"/>
-      <c r="Z22" s="95"/>
-      <c r="AA22" s="68"/>
-      <c r="AB22" s="69"/>
-      <c r="AC22" s="69"/>
-      <c r="AD22" s="70"/>
-      <c r="AE22" s="68"/>
-      <c r="AF22" s="69"/>
-      <c r="AG22" s="69"/>
-      <c r="AH22" s="70"/>
+      <c r="X22" s="103"/>
+      <c r="Y22" s="103"/>
+      <c r="Z22" s="104"/>
+      <c r="AA22" s="85"/>
+      <c r="AB22" s="86"/>
+      <c r="AC22" s="86"/>
+      <c r="AD22" s="87"/>
+      <c r="AE22" s="85"/>
+      <c r="AF22" s="86"/>
+      <c r="AG22" s="86"/>
+      <c r="AH22" s="87"/>
     </row>
     <row r="23" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C23" s="35"/>
@@ -1958,49 +2000,49 @@
         <v>17</v>
       </c>
       <c r="H23" s="21"/>
-      <c r="S23" s="96" t="s">
+      <c r="S23" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="T23" s="97"/>
-      <c r="U23" s="97"/>
-      <c r="V23" s="98"/>
-      <c r="W23" s="73"/>
-      <c r="X23" s="74"/>
-      <c r="Y23" s="74"/>
-      <c r="Z23" s="74"/>
-      <c r="AA23" s="90" t="s">
+      <c r="T23" s="89"/>
+      <c r="U23" s="89"/>
+      <c r="V23" s="90"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="AB23" s="91"/>
-      <c r="AC23" s="91"/>
-      <c r="AD23" s="92"/>
+      <c r="AB23" s="112"/>
+      <c r="AC23" s="112"/>
+      <c r="AD23" s="113"/>
       <c r="AE23" s="41"/>
-      <c r="AF23" s="74"/>
-      <c r="AG23" s="74"/>
-      <c r="AH23" s="75"/>
+      <c r="AF23" s="58"/>
+      <c r="AG23" s="58"/>
+      <c r="AH23" s="59"/>
     </row>
     <row r="24" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C24" s="35"/>
       <c r="D24" s="12"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
-      <c r="S24" s="99" t="s">
+      <c r="S24" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="T24" s="100"/>
-      <c r="U24" s="100"/>
-      <c r="V24" s="101"/>
+      <c r="T24" s="106"/>
+      <c r="U24" s="106"/>
+      <c r="V24" s="107"/>
       <c r="W24" s="41"/>
-      <c r="X24" s="76"/>
-      <c r="Y24" s="76"/>
-      <c r="Z24" s="76"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="60"/>
       <c r="AA24" s="41"/>
-      <c r="AB24" s="76"/>
-      <c r="AC24" s="76"/>
-      <c r="AD24" s="76"/>
+      <c r="AB24" s="60"/>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="60"/>
       <c r="AE24" s="41"/>
-      <c r="AF24" s="76"/>
-      <c r="AG24" s="76"/>
+      <c r="AF24" s="60"/>
+      <c r="AG24" s="60"/>
       <c r="AH24" s="42"/>
     </row>
     <row r="25" spans="3:34" x14ac:dyDescent="0.25">
@@ -2008,31 +2050,31 @@
       <c r="D25" s="34"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="50" t="s">
+      <c r="G25" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="51"/>
+      <c r="H25" s="80"/>
     </row>
     <row r="26" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C26" s="35"/>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="51"/>
+      <c r="H26" s="80"/>
     </row>
     <row r="27" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C27" s="35"/>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="51"/>
+      <c r="H27" s="80"/>
     </row>
     <row r="28" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C28" s="35"/>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="51"/>
+      <c r="H28" s="80"/>
     </row>
     <row r="29" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C29" s="35"/>
@@ -2087,68 +2129,68 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="33"/>
-      <c r="G37" s="52" t="s">
+      <c r="G37" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="H37" s="53"/>
+      <c r="H37" s="71"/>
     </row>
     <row r="38" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="G38" s="53" t="s">
+      <c r="G38" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="53"/>
-      <c r="S38" s="77" t="s">
+      <c r="H38" s="71"/>
+      <c r="S38" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="T38" s="78"/>
-      <c r="U38" s="78"/>
-      <c r="V38" s="78"/>
-      <c r="W38" s="78"/>
-      <c r="X38" s="78"/>
-      <c r="Y38" s="78"/>
-      <c r="Z38" s="78"/>
-      <c r="AA38" s="78"/>
-      <c r="AB38" s="78"/>
-      <c r="AC38" s="78"/>
-      <c r="AD38" s="78"/>
-      <c r="AE38" s="78"/>
-      <c r="AF38" s="78"/>
-      <c r="AG38" s="78"/>
-      <c r="AH38" s="79"/>
+      <c r="T38" s="73"/>
+      <c r="U38" s="73"/>
+      <c r="V38" s="73"/>
+      <c r="W38" s="73"/>
+      <c r="X38" s="73"/>
+      <c r="Y38" s="73"/>
+      <c r="Z38" s="73"/>
+      <c r="AA38" s="73"/>
+      <c r="AB38" s="73"/>
+      <c r="AC38" s="73"/>
+      <c r="AD38" s="73"/>
+      <c r="AE38" s="73"/>
+      <c r="AF38" s="73"/>
+      <c r="AG38" s="73"/>
+      <c r="AH38" s="74"/>
     </row>
     <row r="39" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="G39" s="53" t="s">
+      <c r="G39" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H39" s="53"/>
-      <c r="S39" s="80"/>
-      <c r="T39" s="81"/>
-      <c r="U39" s="81"/>
-      <c r="V39" s="81"/>
-      <c r="W39" s="81"/>
-      <c r="X39" s="81"/>
-      <c r="Y39" s="81"/>
-      <c r="Z39" s="81"/>
-      <c r="AA39" s="81"/>
-      <c r="AB39" s="81"/>
-      <c r="AC39" s="81"/>
-      <c r="AD39" s="81"/>
-      <c r="AE39" s="81"/>
-      <c r="AF39" s="81"/>
-      <c r="AG39" s="81"/>
-      <c r="AH39" s="82"/>
+      <c r="H39" s="71"/>
+      <c r="S39" s="75"/>
+      <c r="T39" s="76"/>
+      <c r="U39" s="76"/>
+      <c r="V39" s="76"/>
+      <c r="W39" s="76"/>
+      <c r="X39" s="76"/>
+      <c r="Y39" s="76"/>
+      <c r="Z39" s="76"/>
+      <c r="AA39" s="76"/>
+      <c r="AB39" s="76"/>
+      <c r="AC39" s="76"/>
+      <c r="AD39" s="76"/>
+      <c r="AE39" s="76"/>
+      <c r="AF39" s="76"/>
+      <c r="AG39" s="76"/>
+      <c r="AH39" s="77"/>
     </row>
     <row r="40" spans="3:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G40" s="53" t="s">
+      <c r="G40" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="H40" s="53"/>
-      <c r="S40" s="107" t="s">
+      <c r="H40" s="71"/>
+      <c r="S40" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="T40" s="111"/>
-      <c r="U40" s="111"/>
-      <c r="V40" s="108"/>
+      <c r="T40" s="65"/>
+      <c r="U40" s="65"/>
+      <c r="V40" s="66"/>
       <c r="W40" s="43"/>
       <c r="X40" s="43"/>
       <c r="Y40" s="43"/>
@@ -2165,10 +2207,10 @@
     <row r="41" spans="3:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G41" s="38"/>
       <c r="H41" s="39"/>
-      <c r="S41" s="109"/>
-      <c r="T41" s="112"/>
-      <c r="U41" s="112"/>
-      <c r="V41" s="110"/>
+      <c r="S41" s="67"/>
+      <c r="T41" s="68"/>
+      <c r="U41" s="68"/>
+      <c r="V41" s="69"/>
       <c r="W41" s="43"/>
       <c r="X41" s="43"/>
       <c r="Y41" s="43"/>
@@ -2185,10 +2227,7 @@
     <row r="42" spans="3:34" x14ac:dyDescent="0.25">
       <c r="G42" s="38"/>
       <c r="H42" s="39"/>
-      <c r="S42" s="72"/>
-      <c r="T42" s="72"/>
-      <c r="U42" s="72"/>
-      <c r="V42" s="113"/>
+      <c r="V42" s="63"/>
       <c r="W42" s="43"/>
       <c r="X42" s="43"/>
       <c r="Y42" s="43"/>
@@ -2205,10 +2244,7 @@
     <row r="43" spans="3:34" x14ac:dyDescent="0.25">
       <c r="G43" s="38"/>
       <c r="H43" s="39"/>
-      <c r="S43" s="72"/>
-      <c r="T43" s="72"/>
-      <c r="U43" s="72"/>
-      <c r="V43" s="113"/>
+      <c r="V43" s="63"/>
       <c r="W43" s="43"/>
       <c r="X43" s="43"/>
       <c r="Y43" s="43"/>
@@ -2225,10 +2261,7 @@
     <row r="44" spans="3:34" x14ac:dyDescent="0.25">
       <c r="G44" s="38"/>
       <c r="H44" s="40"/>
-      <c r="S44" s="72"/>
-      <c r="T44" s="72"/>
-      <c r="U44" s="72"/>
-      <c r="V44" s="113"/>
+      <c r="V44" s="63"/>
       <c r="W44" s="43"/>
       <c r="X44" s="43"/>
       <c r="Y44" s="43"/>
@@ -2243,10 +2276,7 @@
       <c r="AH44" s="43"/>
     </row>
     <row r="45" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="S45" s="72"/>
-      <c r="T45" s="72"/>
-      <c r="U45" s="72"/>
-      <c r="V45" s="113"/>
+      <c r="V45" s="63"/>
       <c r="W45" s="43"/>
       <c r="X45" s="43"/>
       <c r="Y45" s="43"/>
@@ -2261,10 +2291,7 @@
       <c r="AH45" s="43"/>
     </row>
     <row r="46" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="S46" s="72"/>
-      <c r="T46" s="72"/>
-      <c r="U46" s="72"/>
-      <c r="V46" s="113"/>
+      <c r="V46" s="63"/>
       <c r="W46" s="43"/>
       <c r="X46" s="43"/>
       <c r="Y46" s="43"/>
@@ -2279,11 +2306,7 @@
       <c r="AH46" s="43"/>
     </row>
     <row r="47" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="R47" s="72"/>
-      <c r="S47" s="72"/>
-      <c r="T47" s="72"/>
-      <c r="U47" s="72"/>
-      <c r="V47" s="113"/>
+      <c r="V47" s="63"/>
       <c r="W47" s="43"/>
       <c r="X47" s="43"/>
       <c r="Y47" s="43"/>
@@ -2298,12 +2321,12 @@
       <c r="AH47" s="43"/>
     </row>
     <row r="48" spans="3:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S48" s="114">
+      <c r="S48" s="70">
         <v>1</v>
       </c>
-      <c r="T48" s="114"/>
-      <c r="U48" s="114"/>
-      <c r="V48" s="114"/>
+      <c r="T48" s="70"/>
+      <c r="U48" s="70"/>
+      <c r="V48" s="70"/>
       <c r="W48" s="43"/>
       <c r="X48" s="43"/>
       <c r="Y48" s="43"/>
@@ -2318,76 +2341,41 @@
       <c r="AH48" s="43"/>
     </row>
     <row r="49" spans="19:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S49" s="114"/>
-      <c r="T49" s="114"/>
-      <c r="U49" s="114"/>
-      <c r="V49" s="114"/>
+      <c r="S49" s="70"/>
+      <c r="T49" s="70"/>
+      <c r="U49" s="70"/>
+      <c r="V49" s="70"/>
     </row>
     <row r="57" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S57" s="114">
+      <c r="S57" s="70">
         <v>2</v>
       </c>
-      <c r="T57" s="114"/>
-      <c r="U57" s="114"/>
-      <c r="V57" s="114"/>
+      <c r="T57" s="70"/>
+      <c r="U57" s="70"/>
+      <c r="V57" s="70"/>
     </row>
     <row r="58" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S58" s="114"/>
-      <c r="T58" s="114"/>
-      <c r="U58" s="114"/>
-      <c r="V58" s="114"/>
+      <c r="S58" s="70"/>
+      <c r="T58" s="70"/>
+      <c r="U58" s="70"/>
+      <c r="V58" s="70"/>
     </row>
     <row r="61" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S61" s="114">
+      <c r="S61" s="70">
         <v>3</v>
       </c>
-      <c r="T61" s="114"/>
-      <c r="U61" s="114"/>
-      <c r="V61" s="114"/>
+      <c r="T61" s="70"/>
+      <c r="U61" s="70"/>
+      <c r="V61" s="70"/>
     </row>
     <row r="62" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S62" s="114"/>
-      <c r="T62" s="114"/>
-      <c r="U62" s="114"/>
-      <c r="V62" s="114"/>
+      <c r="S62" s="70"/>
+      <c r="T62" s="70"/>
+      <c r="U62" s="70"/>
+      <c r="V62" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="S40:V41"/>
-    <mergeCell ref="S48:V49"/>
-    <mergeCell ref="S57:V58"/>
-    <mergeCell ref="S61:V62"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="S2:AH3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AA19:AD19"/>
-    <mergeCell ref="S38:AH39"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="W21:Z21"/>
-    <mergeCell ref="S23:V23"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="S15:AH16"/>
-    <mergeCell ref="AE17:AH17"/>
-    <mergeCell ref="S17:V17"/>
-    <mergeCell ref="W17:Z17"/>
-    <mergeCell ref="AA17:AD17"/>
-    <mergeCell ref="S21:V21"/>
-    <mergeCell ref="AE18:AH18"/>
-    <mergeCell ref="AE19:AH19"/>
-    <mergeCell ref="AE20:AH20"/>
-    <mergeCell ref="AE21:AH21"/>
+  <mergeCells count="46">
     <mergeCell ref="AE22:AH22"/>
     <mergeCell ref="AA18:AD18"/>
     <mergeCell ref="W22:Z22"/>
@@ -2398,6 +2386,42 @@
     <mergeCell ref="AA22:AD22"/>
     <mergeCell ref="W19:Z19"/>
     <mergeCell ref="W20:Z20"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="S15:AH16"/>
+    <mergeCell ref="AE17:AH17"/>
+    <mergeCell ref="S17:V17"/>
+    <mergeCell ref="W17:Z17"/>
+    <mergeCell ref="AA17:AD17"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="S38:AH39"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="S2:AH3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AA19:AD19"/>
+    <mergeCell ref="W21:Z21"/>
+    <mergeCell ref="S23:V23"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="S21:V21"/>
+    <mergeCell ref="AE18:AH18"/>
+    <mergeCell ref="AE19:AH19"/>
+    <mergeCell ref="AE20:AH20"/>
+    <mergeCell ref="AE21:AH21"/>
+    <mergeCell ref="S40:V41"/>
+    <mergeCell ref="S48:V49"/>
+    <mergeCell ref="S57:V58"/>
+    <mergeCell ref="S61:V62"/>
+    <mergeCell ref="G40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
AMBL y buscar por ID, class Producto
</commit_message>
<xml_diff>
--- a/Diagrama Proyecto Lab 2.xlsx
+++ b/Diagrama Proyecto Lab 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://frgputneduar-my.sharepoint.com/personal/agustin_bernal_alumnos_frgp_utn_edu_ar/Documents/Escritorio/Proyecto LAB II/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aby\Desktop\Repositorio Labo2\Proyecto-Final-LAB-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:1_{D72C21AE-0112-4E12-ABC5-1399829BE6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{372A2EA0-EA6B-441F-B820-E0AB1493EE44}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE26A52-AE6C-4F8A-9A48-C07BFC78ABA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{114F25F1-BAA8-49DE-8C7A-F4FC53EA1D42}"/>
+    <workbookView xWindow="5370" yWindow="1485" windowWidth="21600" windowHeight="11295" xr2:uid="{114F25F1-BAA8-49DE-8C7A-F4FC53EA1D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Menu Principal</t>
   </si>
@@ -264,13 +264,37 @@
   </si>
   <si>
     <t xml:space="preserve">    Fecha </t>
+  </si>
+  <si>
+    <t>Listar mesas no</t>
+  </si>
+  <si>
+    <t>reservadas</t>
+  </si>
+  <si>
+    <t>Buscar reserva</t>
+  </si>
+  <si>
+    <t>por fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar cliente </t>
+  </si>
+  <si>
+    <t>por nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con un algoritmo que enseñó kloster en  una clase, me gustaria hacer una funcion en productos que muestre los productos </t>
+  </si>
+  <si>
+    <t>tal vez por cantidad y que se muestren de menor precio a mayor, es una idea que tengo y que voy a probar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +366,13 @@
     <font>
       <sz val="11"/>
       <color theme="2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -632,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -697,6 +728,10 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,31 +756,13 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,25 +774,46 @@
     <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -799,9 +837,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -847,9 +882,7 @@
     <xf numFmtId="0" fontId="8" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,10 +1084,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1376,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767514CD-FE6A-45D5-A469-684433B41042}">
   <dimension ref="A2:AH62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19:AH19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,28 +1417,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="S2" s="72" t="s">
+      <c r="B2" s="95"/>
+      <c r="S2" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="74"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
+      <c r="AG2" s="88"/>
+      <c r="AH2" s="89"/>
     </row>
     <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1424,22 +1453,22 @@
         <v>5</v>
       </c>
       <c r="H3" s="25"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="76"/>
-      <c r="AC3" s="76"/>
-      <c r="AD3" s="76"/>
-      <c r="AE3" s="76"/>
-      <c r="AF3" s="76"/>
-      <c r="AG3" s="76"/>
-      <c r="AH3" s="77"/>
+      <c r="S3" s="90"/>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="91"/>
+      <c r="X3" s="91"/>
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="91"/>
+      <c r="AA3" s="91"/>
+      <c r="AB3" s="91"/>
+      <c r="AC3" s="91"/>
+      <c r="AD3" s="91"/>
+      <c r="AE3" s="91"/>
+      <c r="AF3" s="91"/>
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="92"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -1468,30 +1497,30 @@
         <v>15</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="S5" s="78" t="s">
+      <c r="S5" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="78"/>
+      <c r="T5" s="76"/>
       <c r="U5" s="27"/>
-      <c r="V5" s="78" t="s">
+      <c r="V5" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="W5" s="78"/>
+      <c r="W5" s="76"/>
       <c r="X5" s="27"/>
-      <c r="Y5" s="78" t="s">
+      <c r="Y5" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="Z5" s="78"/>
+      <c r="Z5" s="76"/>
       <c r="AA5" s="27"/>
-      <c r="AB5" s="78" t="s">
+      <c r="AB5" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="AC5" s="78"/>
+      <c r="AC5" s="76"/>
       <c r="AD5" s="27"/>
-      <c r="AE5" s="78" t="s">
+      <c r="AE5" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="AF5" s="78"/>
+      <c r="AF5" s="76"/>
       <c r="AG5" s="27"/>
       <c r="AH5" s="27"/>
     </row>
@@ -1527,7 +1556,7 @@
       <c r="AB6" s="46"/>
       <c r="AC6" s="47"/>
       <c r="AD6" s="27"/>
-      <c r="AE6" s="114" t="s">
+      <c r="AE6" s="64" t="s">
         <v>68</v>
       </c>
       <c r="AF6" s="47"/>
@@ -1535,10 +1564,10 @@
       <c r="AH6" s="27"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="36"/>
       <c r="D7" s="2"/>
       <c r="E7" s="8"/>
@@ -1573,10 +1602,10 @@
       <c r="AH7" s="27"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="94"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="35"/>
       <c r="D8" s="2"/>
       <c r="E8" s="8"/>
@@ -1685,6 +1714,16 @@
         <v>10</v>
       </c>
       <c r="H11" s="19"/>
+      <c r="I11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
       <c r="S11" s="44" t="s">
         <v>37</v>
       </c>
@@ -1716,6 +1755,15 @@
         <v>11</v>
       </c>
       <c r="H12" s="19"/>
+      <c r="I12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
       <c r="S12" s="45" t="s">
         <v>43</v>
       </c>
@@ -1796,24 +1844,24 @@
         <v>12</v>
       </c>
       <c r="H15" s="19"/>
-      <c r="S15" s="72" t="s">
+      <c r="S15" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="T15" s="73"/>
-      <c r="U15" s="73"/>
-      <c r="V15" s="73"/>
-      <c r="W15" s="73"/>
-      <c r="X15" s="73"/>
-      <c r="Y15" s="73"/>
-      <c r="Z15" s="73"/>
-      <c r="AA15" s="73"/>
-      <c r="AB15" s="73"/>
-      <c r="AC15" s="73"/>
-      <c r="AD15" s="73"/>
-      <c r="AE15" s="73"/>
-      <c r="AF15" s="73"/>
-      <c r="AG15" s="73"/>
-      <c r="AH15" s="74"/>
+      <c r="T15" s="88"/>
+      <c r="U15" s="88"/>
+      <c r="V15" s="88"/>
+      <c r="W15" s="88"/>
+      <c r="X15" s="88"/>
+      <c r="Y15" s="88"/>
+      <c r="Z15" s="88"/>
+      <c r="AA15" s="88"/>
+      <c r="AB15" s="88"/>
+      <c r="AC15" s="88"/>
+      <c r="AD15" s="88"/>
+      <c r="AE15" s="88"/>
+      <c r="AF15" s="88"/>
+      <c r="AG15" s="88"/>
+      <c r="AH15" s="89"/>
     </row>
     <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="35"/>
@@ -1823,22 +1871,22 @@
         <v>13</v>
       </c>
       <c r="H16" s="19"/>
-      <c r="S16" s="75"/>
-      <c r="T16" s="76"/>
-      <c r="U16" s="76"/>
-      <c r="V16" s="76"/>
-      <c r="W16" s="76"/>
-      <c r="X16" s="76"/>
-      <c r="Y16" s="76"/>
-      <c r="Z16" s="76"/>
-      <c r="AA16" s="76"/>
-      <c r="AB16" s="76"/>
-      <c r="AC16" s="76"/>
-      <c r="AD16" s="76"/>
-      <c r="AE16" s="76"/>
-      <c r="AF16" s="76"/>
-      <c r="AG16" s="76"/>
-      <c r="AH16" s="77"/>
+      <c r="S16" s="90"/>
+      <c r="T16" s="91"/>
+      <c r="U16" s="91"/>
+      <c r="V16" s="91"/>
+      <c r="W16" s="91"/>
+      <c r="X16" s="91"/>
+      <c r="Y16" s="91"/>
+      <c r="Z16" s="91"/>
+      <c r="AA16" s="91"/>
+      <c r="AB16" s="91"/>
+      <c r="AC16" s="91"/>
+      <c r="AD16" s="91"/>
+      <c r="AE16" s="91"/>
+      <c r="AF16" s="91"/>
+      <c r="AG16" s="91"/>
+      <c r="AH16" s="92"/>
     </row>
     <row r="17" spans="3:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="35"/>
@@ -1848,30 +1896,30 @@
         <v>17</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="S17" s="97" t="s">
+      <c r="S17" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="T17" s="97"/>
-      <c r="U17" s="97"/>
-      <c r="V17" s="97"/>
-      <c r="W17" s="97" t="s">
+      <c r="T17" s="100"/>
+      <c r="U17" s="100"/>
+      <c r="V17" s="100"/>
+      <c r="W17" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="X17" s="97"/>
-      <c r="Y17" s="97"/>
-      <c r="Z17" s="97"/>
-      <c r="AA17" s="97" t="s">
+      <c r="X17" s="100"/>
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="100"/>
+      <c r="AA17" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="AB17" s="97"/>
-      <c r="AC17" s="97"/>
-      <c r="AD17" s="97"/>
-      <c r="AE17" s="97" t="s">
+      <c r="AB17" s="100"/>
+      <c r="AC17" s="100"/>
+      <c r="AD17" s="100"/>
+      <c r="AE17" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="AF17" s="97"/>
-      <c r="AG17" s="97"/>
-      <c r="AH17" s="97"/>
+      <c r="AF17" s="100"/>
+      <c r="AG17" s="100"/>
+      <c r="AH17" s="100"/>
     </row>
     <row r="18" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C18" s="35"/>
@@ -1881,16 +1929,16 @@
       <c r="H18" s="27"/>
       <c r="S18" s="57"/>
       <c r="W18" s="41"/>
-      <c r="AA18" s="99" t="s">
+      <c r="AA18" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="AB18" s="100"/>
-      <c r="AC18" s="100"/>
-      <c r="AD18" s="101"/>
-      <c r="AE18" s="85"/>
-      <c r="AF18" s="86"/>
-      <c r="AG18" s="86"/>
-      <c r="AH18" s="87"/>
+      <c r="AB18" s="102"/>
+      <c r="AC18" s="102"/>
+      <c r="AD18" s="103"/>
+      <c r="AE18" s="80"/>
+      <c r="AF18" s="81"/>
+      <c r="AG18" s="81"/>
+      <c r="AH18" s="82"/>
     </row>
     <row r="19" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C19" s="35"/>
@@ -1901,24 +1949,35 @@
         <v>18</v>
       </c>
       <c r="H19" s="21"/>
+      <c r="I19" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+      <c r="N19" s="65"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
       <c r="S19" s="41"/>
       <c r="T19" s="60"/>
       <c r="U19" s="60"/>
       <c r="V19" s="42"/>
-      <c r="W19" s="85"/>
-      <c r="X19" s="86"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="87"/>
-      <c r="AA19" s="81" t="s">
+      <c r="W19" s="80"/>
+      <c r="X19" s="81"/>
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="82"/>
+      <c r="AA19" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="AB19" s="82"/>
-      <c r="AC19" s="82"/>
-      <c r="AD19" s="83"/>
-      <c r="AE19" s="85"/>
-      <c r="AF19" s="86"/>
-      <c r="AG19" s="86"/>
-      <c r="AH19" s="87"/>
+      <c r="AB19" s="78"/>
+      <c r="AC19" s="78"/>
+      <c r="AD19" s="79"/>
+      <c r="AE19" s="80"/>
+      <c r="AF19" s="81"/>
+      <c r="AG19" s="81"/>
+      <c r="AH19" s="82"/>
     </row>
     <row r="20" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C20" s="35"/>
@@ -1927,24 +1986,32 @@
         <v>19</v>
       </c>
       <c r="H20" s="21"/>
-      <c r="S20" s="85"/>
-      <c r="T20" s="86"/>
-      <c r="U20" s="86"/>
-      <c r="V20" s="87"/>
-      <c r="W20" s="85"/>
-      <c r="X20" s="86"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="87"/>
-      <c r="AA20" s="108" t="s">
+      <c r="I20" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="S20" s="80"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="81"/>
+      <c r="V20" s="82"/>
+      <c r="W20" s="80"/>
+      <c r="X20" s="81"/>
+      <c r="Y20" s="81"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="AB20" s="109"/>
-      <c r="AC20" s="109"/>
-      <c r="AD20" s="110"/>
-      <c r="AE20" s="85"/>
-      <c r="AF20" s="86"/>
-      <c r="AG20" s="86"/>
-      <c r="AH20" s="87"/>
+      <c r="AB20" s="111"/>
+      <c r="AC20" s="111"/>
+      <c r="AD20" s="112"/>
+      <c r="AE20" s="80"/>
+      <c r="AF20" s="81"/>
+      <c r="AG20" s="81"/>
+      <c r="AH20" s="82"/>
     </row>
     <row r="21" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C21" s="35"/>
@@ -1953,22 +2020,22 @@
         <v>20</v>
       </c>
       <c r="H21" s="21"/>
-      <c r="S21" s="98"/>
-      <c r="T21" s="98"/>
-      <c r="U21" s="98"/>
-      <c r="V21" s="98"/>
-      <c r="W21" s="85"/>
-      <c r="X21" s="86"/>
-      <c r="Y21" s="86"/>
-      <c r="Z21" s="87"/>
-      <c r="AA21" s="85"/>
-      <c r="AB21" s="86"/>
-      <c r="AC21" s="86"/>
-      <c r="AD21" s="87"/>
-      <c r="AE21" s="85"/>
-      <c r="AF21" s="86"/>
-      <c r="AG21" s="86"/>
-      <c r="AH21" s="87"/>
+      <c r="S21" s="86"/>
+      <c r="T21" s="86"/>
+      <c r="U21" s="86"/>
+      <c r="V21" s="86"/>
+      <c r="W21" s="80"/>
+      <c r="X21" s="81"/>
+      <c r="Y21" s="81"/>
+      <c r="Z21" s="82"/>
+      <c r="AA21" s="80"/>
+      <c r="AB21" s="81"/>
+      <c r="AC21" s="81"/>
+      <c r="AD21" s="82"/>
+      <c r="AE21" s="80"/>
+      <c r="AF21" s="81"/>
+      <c r="AG21" s="81"/>
+      <c r="AH21" s="82"/>
     </row>
     <row r="22" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C22" s="35"/>
@@ -1977,21 +2044,31 @@
         <v>8</v>
       </c>
       <c r="H22" s="29"/>
+      <c r="I22" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
       <c r="S22" s="41"/>
-      <c r="W22" s="102" t="s">
+      <c r="W22" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="X22" s="103"/>
-      <c r="Y22" s="103"/>
-      <c r="Z22" s="104"/>
-      <c r="AA22" s="85"/>
-      <c r="AB22" s="86"/>
-      <c r="AC22" s="86"/>
-      <c r="AD22" s="87"/>
-      <c r="AE22" s="85"/>
-      <c r="AF22" s="86"/>
-      <c r="AG22" s="86"/>
-      <c r="AH22" s="87"/>
+      <c r="X22" s="105"/>
+      <c r="Y22" s="105"/>
+      <c r="Z22" s="106"/>
+      <c r="AA22" s="80"/>
+      <c r="AB22" s="81"/>
+      <c r="AC22" s="81"/>
+      <c r="AD22" s="82"/>
+      <c r="AE22" s="80"/>
+      <c r="AF22" s="81"/>
+      <c r="AG22" s="81"/>
+      <c r="AH22" s="82"/>
     </row>
     <row r="23" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C23" s="35"/>
@@ -2000,22 +2077,30 @@
         <v>17</v>
       </c>
       <c r="H23" s="21"/>
-      <c r="S23" s="88" t="s">
+      <c r="I23" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
+      <c r="S23" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="T23" s="89"/>
-      <c r="U23" s="89"/>
-      <c r="V23" s="90"/>
+      <c r="T23" s="84"/>
+      <c r="U23" s="84"/>
+      <c r="V23" s="85"/>
       <c r="W23" s="57"/>
       <c r="X23" s="58"/>
       <c r="Y23" s="58"/>
       <c r="Z23" s="58"/>
-      <c r="AA23" s="111" t="s">
+      <c r="AA23" s="113" t="s">
         <v>63</v>
       </c>
-      <c r="AB23" s="112"/>
-      <c r="AC23" s="112"/>
-      <c r="AD23" s="113"/>
+      <c r="AB23" s="114"/>
+      <c r="AC23" s="114"/>
+      <c r="AD23" s="115"/>
       <c r="AE23" s="41"/>
       <c r="AF23" s="58"/>
       <c r="AG23" s="58"/>
@@ -2026,12 +2111,12 @@
       <c r="D24" s="12"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
-      <c r="S24" s="105" t="s">
+      <c r="S24" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="T24" s="106"/>
-      <c r="U24" s="106"/>
-      <c r="V24" s="107"/>
+      <c r="T24" s="108"/>
+      <c r="U24" s="108"/>
+      <c r="V24" s="109"/>
       <c r="W24" s="41"/>
       <c r="X24" s="60"/>
       <c r="Y24" s="60"/>
@@ -2050,31 +2135,37 @@
       <c r="D25" s="34"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="79" t="s">
+      <c r="G25" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="80"/>
+      <c r="H25" s="75"/>
     </row>
     <row r="26" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C26" s="35"/>
-      <c r="G26" s="79" t="s">
+      <c r="G26" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="80"/>
+      <c r="H26" s="75"/>
     </row>
     <row r="27" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C27" s="35"/>
-      <c r="G27" s="79" t="s">
+      <c r="G27" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="80"/>
+      <c r="H27" s="75"/>
+      <c r="S27" s="116" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C28" s="35"/>
-      <c r="G28" s="79" t="s">
+      <c r="G28" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="80"/>
+      <c r="H28" s="75"/>
+      <c r="S28" s="116" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="29" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C29" s="35"/>
@@ -2129,68 +2220,68 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="33"/>
-      <c r="G37" s="84" t="s">
+      <c r="G37" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="H37" s="71"/>
+      <c r="H37" s="73"/>
     </row>
     <row r="38" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="G38" s="71" t="s">
+      <c r="G38" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="71"/>
-      <c r="S38" s="72" t="s">
+      <c r="H38" s="73"/>
+      <c r="S38" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="T38" s="73"/>
-      <c r="U38" s="73"/>
-      <c r="V38" s="73"/>
-      <c r="W38" s="73"/>
-      <c r="X38" s="73"/>
-      <c r="Y38" s="73"/>
-      <c r="Z38" s="73"/>
-      <c r="AA38" s="73"/>
-      <c r="AB38" s="73"/>
-      <c r="AC38" s="73"/>
-      <c r="AD38" s="73"/>
-      <c r="AE38" s="73"/>
-      <c r="AF38" s="73"/>
-      <c r="AG38" s="73"/>
-      <c r="AH38" s="74"/>
+      <c r="T38" s="88"/>
+      <c r="U38" s="88"/>
+      <c r="V38" s="88"/>
+      <c r="W38" s="88"/>
+      <c r="X38" s="88"/>
+      <c r="Y38" s="88"/>
+      <c r="Z38" s="88"/>
+      <c r="AA38" s="88"/>
+      <c r="AB38" s="88"/>
+      <c r="AC38" s="88"/>
+      <c r="AD38" s="88"/>
+      <c r="AE38" s="88"/>
+      <c r="AF38" s="88"/>
+      <c r="AG38" s="88"/>
+      <c r="AH38" s="89"/>
     </row>
     <row r="39" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="G39" s="71" t="s">
+      <c r="G39" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="H39" s="71"/>
-      <c r="S39" s="75"/>
-      <c r="T39" s="76"/>
-      <c r="U39" s="76"/>
-      <c r="V39" s="76"/>
-      <c r="W39" s="76"/>
-      <c r="X39" s="76"/>
-      <c r="Y39" s="76"/>
-      <c r="Z39" s="76"/>
-      <c r="AA39" s="76"/>
-      <c r="AB39" s="76"/>
-      <c r="AC39" s="76"/>
-      <c r="AD39" s="76"/>
-      <c r="AE39" s="76"/>
-      <c r="AF39" s="76"/>
-      <c r="AG39" s="76"/>
-      <c r="AH39" s="77"/>
+      <c r="H39" s="73"/>
+      <c r="S39" s="90"/>
+      <c r="T39" s="91"/>
+      <c r="U39" s="91"/>
+      <c r="V39" s="91"/>
+      <c r="W39" s="91"/>
+      <c r="X39" s="91"/>
+      <c r="Y39" s="91"/>
+      <c r="Z39" s="91"/>
+      <c r="AA39" s="91"/>
+      <c r="AB39" s="91"/>
+      <c r="AC39" s="91"/>
+      <c r="AD39" s="91"/>
+      <c r="AE39" s="91"/>
+      <c r="AF39" s="91"/>
+      <c r="AG39" s="91"/>
+      <c r="AH39" s="92"/>
     </row>
     <row r="40" spans="3:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G40" s="71" t="s">
+      <c r="G40" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="H40" s="71"/>
-      <c r="S40" s="64" t="s">
+      <c r="H40" s="73"/>
+      <c r="S40" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="T40" s="65"/>
-      <c r="U40" s="65"/>
-      <c r="V40" s="66"/>
+      <c r="T40" s="67"/>
+      <c r="U40" s="67"/>
+      <c r="V40" s="68"/>
       <c r="W40" s="43"/>
       <c r="X40" s="43"/>
       <c r="Y40" s="43"/>
@@ -2207,10 +2298,10 @@
     <row r="41" spans="3:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G41" s="38"/>
       <c r="H41" s="39"/>
-      <c r="S41" s="67"/>
-      <c r="T41" s="68"/>
-      <c r="U41" s="68"/>
-      <c r="V41" s="69"/>
+      <c r="S41" s="69"/>
+      <c r="T41" s="70"/>
+      <c r="U41" s="70"/>
+      <c r="V41" s="71"/>
       <c r="W41" s="43"/>
       <c r="X41" s="43"/>
       <c r="Y41" s="43"/>
@@ -2321,12 +2412,12 @@
       <c r="AH47" s="43"/>
     </row>
     <row r="48" spans="3:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S48" s="70">
+      <c r="S48" s="72">
         <v>1</v>
       </c>
-      <c r="T48" s="70"/>
-      <c r="U48" s="70"/>
-      <c r="V48" s="70"/>
+      <c r="T48" s="72"/>
+      <c r="U48" s="72"/>
+      <c r="V48" s="72"/>
       <c r="W48" s="43"/>
       <c r="X48" s="43"/>
       <c r="Y48" s="43"/>
@@ -2341,38 +2432,38 @@
       <c r="AH48" s="43"/>
     </row>
     <row r="49" spans="19:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S49" s="70"/>
-      <c r="T49" s="70"/>
-      <c r="U49" s="70"/>
-      <c r="V49" s="70"/>
+      <c r="S49" s="72"/>
+      <c r="T49" s="72"/>
+      <c r="U49" s="72"/>
+      <c r="V49" s="72"/>
     </row>
     <row r="57" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S57" s="70">
+      <c r="S57" s="72">
         <v>2</v>
       </c>
-      <c r="T57" s="70"/>
-      <c r="U57" s="70"/>
-      <c r="V57" s="70"/>
+      <c r="T57" s="72"/>
+      <c r="U57" s="72"/>
+      <c r="V57" s="72"/>
     </row>
     <row r="58" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S58" s="70"/>
-      <c r="T58" s="70"/>
-      <c r="U58" s="70"/>
-      <c r="V58" s="70"/>
+      <c r="S58" s="72"/>
+      <c r="T58" s="72"/>
+      <c r="U58" s="72"/>
+      <c r="V58" s="72"/>
     </row>
     <row r="61" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S61" s="70">
+      <c r="S61" s="72">
         <v>3</v>
       </c>
-      <c r="T61" s="70"/>
-      <c r="U61" s="70"/>
-      <c r="V61" s="70"/>
+      <c r="T61" s="72"/>
+      <c r="U61" s="72"/>
+      <c r="V61" s="72"/>
     </row>
     <row r="62" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S62" s="70"/>
-      <c r="T62" s="70"/>
-      <c r="U62" s="70"/>
-      <c r="V62" s="70"/>
+      <c r="S62" s="72"/>
+      <c r="T62" s="72"/>
+      <c r="U62" s="72"/>
+      <c r="V62" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="46">
@@ -2386,6 +2477,10 @@
     <mergeCell ref="AA22:AD22"/>
     <mergeCell ref="W19:Z19"/>
     <mergeCell ref="W20:Z20"/>
+    <mergeCell ref="AE18:AH18"/>
+    <mergeCell ref="AE19:AH19"/>
+    <mergeCell ref="AE20:AH20"/>
+    <mergeCell ref="AE21:AH21"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A7:B7"/>
@@ -2395,16 +2490,16 @@
     <mergeCell ref="W17:Z17"/>
     <mergeCell ref="AA17:AD17"/>
     <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="S2:AH3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="S38:AH39"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G39:H39"/>
-    <mergeCell ref="S2:AH3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="AB5:AC5"/>
@@ -2413,10 +2508,6 @@
     <mergeCell ref="S23:V23"/>
     <mergeCell ref="S20:V20"/>
     <mergeCell ref="S21:V21"/>
-    <mergeCell ref="AE18:AH18"/>
-    <mergeCell ref="AE19:AH19"/>
-    <mergeCell ref="AE20:AH20"/>
-    <mergeCell ref="AE21:AH21"/>
     <mergeCell ref="S40:V41"/>
     <mergeCell ref="S48:V49"/>
     <mergeCell ref="S57:V58"/>

</xml_diff>